<commit_message>
Durio ile konuşma sonrası düzeltmeler.
</commit_message>
<xml_diff>
--- a/pad/freq.xlsx
+++ b/pad/freq.xlsx
@@ -19,8 +19,72 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Andale Mono"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">üç konulu makale sayısı</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Andale Mono"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">dört konulu makale sayısı</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Yukarıda 3 sayısından 3 tane var</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Yukarırda 4 sayısından 1 tane var</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t xml:space="preserve">Input Table</t>
   </si>
@@ -196,40 +260,49 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Next Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counting all occurences</t>
+    <t xml:space="preserve">Durio: Stattistical summary column F </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAT TABLE(VERIFIED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of topic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of paper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cum %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.75%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of papers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(p1,p2,p3,p4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suffi</t>
   </si>
   <si>
     <t xml:space="preserve">Topic</t>
   </si>
   <si>
-    <t xml:space="preserve">How many paper about t_x on the above table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freq: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cumulative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Question: Which alternative is right for the next table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counting first occurence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How many paper about t_x in the first occurence on the above table</t>
+    <t xml:space="preserve">Number of paper in corpus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">half of the papers speaks about the topic 2</t>
   </si>
 </sst>
 </file>
@@ -240,7 +313,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="%0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -264,6 +337,21 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Andale Mono"/>
@@ -271,14 +359,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Andale Mono"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF18A303"/>
       <name val="Andale Mono"/>
@@ -291,6 +371,26 @@
       <name val="Andale Mono"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF18A303"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Andale Mono"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -360,7 +460,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,15 +481,23 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -405,19 +513,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,23 +621,23 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="63.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="60.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,7 +648,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -551,7 +671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -567,14 +687,14 @@
       <c r="E3" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -590,14 +710,14 @@
       <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -613,14 +733,14 @@
       <c r="E5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -636,212 +756,173 @@
       <c r="E6" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>18</v>
-      </c>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="11" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B14" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="D14" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="F14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="13" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="21.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B21" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="12" t="n">
-        <f aca="false">B12/$B$16</f>
-        <v>0.307692307692308</v>
-      </c>
-      <c r="D12" s="12" t="n">
-        <f aca="false">C12</f>
-        <v>0.307692307692308</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="C21" s="9" t="n">
+        <f aca="false">B21/$C$18</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B22" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="12" t="n">
-        <f aca="false">B13/$B$16</f>
-        <v>0.153846153846154</v>
-      </c>
-      <c r="D13" s="12" t="n">
-        <f aca="false">C13+D12</f>
-        <v>0.461538461538462</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="C22" s="9" t="n">
+        <f aca="false">B22/$C$18</f>
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C14" s="12" t="n">
-        <f aca="false">B14/$B$16</f>
-        <v>0.230769230769231</v>
-      </c>
-      <c r="D14" s="12" t="n">
-        <f aca="false">C14+D13</f>
-        <v>0.692307692307692</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="C23" s="9" t="n">
+        <f aca="false">B23/$C$18</f>
+        <v>0.75</v>
+      </c>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C15" s="12" t="n">
-        <f aca="false">B15/$B$16</f>
-        <v>0.307692307692308</v>
-      </c>
-      <c r="D15" s="12" t="n">
-        <f aca="false">C15+D14</f>
+      <c r="C24" s="9" t="n">
+        <f aca="false">B24/$C$18</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="n">
-        <f aca="false">SUM(B12:B15)</f>
-        <v>13</v>
-      </c>
-      <c r="C16" s="12"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="12" t="n">
-        <f aca="false">B22/$B$26</f>
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="12" t="n">
-        <f aca="false">C22</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="12" t="n">
-        <f aca="false">B23/$B$26</f>
-        <v>0.25</v>
-      </c>
-      <c r="D23" s="12" t="n">
-        <f aca="false">C23+D22</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C24" s="12" t="n">
-        <f aca="false">B24/$B$26</f>
-        <v>0.25</v>
-      </c>
-      <c r="D24" s="12" t="n">
-        <f aca="false">C24+D23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" s="12" t="n">
-        <f aca="false">B25/$B$26</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="12" t="n">
-        <f aca="false">C25+D24</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="n">
-        <f aca="false">SUM(B22:B25)</f>
-        <v>4</v>
-      </c>
-      <c r="C26" s="12"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -851,5 +932,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>